<commit_message>
OW-438 make unit tests passed with the latest portfolio mapping changes
</commit_message>
<xml_diff>
--- a/src/test/resources/portfolio/OneZCS.xlsx
+++ b/src/test/resources/portfolio/OneZCS.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="127">
   <si>
     <t xml:space="preserve">Value Date</t>
   </si>
@@ -331,6 +331,9 @@
     <t xml:space="preserve">Trade Date</t>
   </si>
   <si>
+    <t xml:space="preserve">Trade Status</t>
+  </si>
+  <si>
     <t xml:space="preserve">LEG1_NOTIONALXG</t>
   </si>
   <si>
@@ -440,6 +443,9 @@
   </si>
   <si>
     <t xml:space="preserve">95,000,000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`</t>
   </si>
 </sst>
 </file>
@@ -451,7 +457,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY/MM/DD"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -479,6 +485,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -523,7 +534,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -536,7 +547,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,59 +584,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="51" min="50" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="57" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="51" min="50" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="57" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,49 +831,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="38" min="37" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="38" min="37" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1023,61 +1038,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="52" min="51" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="58" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="52" min="51" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="56" min="56" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="57" min="57" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="58" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1277,50 +1288,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="46" min="45" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="40" min="39" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="46" min="45" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,33 +1495,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,67 +1627,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BE7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB8" activeCellId="0" sqref="AB8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="44" min="43" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="51" min="50" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="55" min="54" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.8520408163265"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.57142857142857"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.54081632653061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.51530612244898"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="46" min="45" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="0" width="23.2448979591837"/>
+    <col collapsed="false" hidden="false" max="50" min="50" style="0" width="23.5255102040816"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="10.6020408163265"/>
+    <col collapsed="false" hidden="false" max="53" min="52" style="0" width="18.9336734693878"/>
+    <col collapsed="false" hidden="false" max="55" min="54" style="0" width="25.6020408163265"/>
+    <col collapsed="false" hidden="false" max="57" min="56" style="0" width="23.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="58" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1696,306 +1707,323 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="T1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="W1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="X1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="Y1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="Z1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="AB1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AC1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AD1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AE1" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AF1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AG1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AH1" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AI1" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AJ1" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AK1" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AL1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AM1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AN1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AO1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AP1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AQ1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AR1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AS1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AT1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="0" t="s">
+      <c r="AU1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AV1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="0" t="s">
+      <c r="AW1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="0" t="s">
+      <c r="AX1" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="0" t="s">
+      <c r="AY1" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY1" s="0" t="s">
+      <c r="AZ1" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="AZ1" s="0" t="s">
+      <c r="BA1" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="BA1" s="0" t="s">
+      <c r="BB1" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="BB1" s="0" t="s">
+      <c r="BC1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="BC1" s="0" t="s">
+      <c r="BD1" s="0" t="s">
         <v>93</v>
       </c>
+      <c r="BE1" s="0" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
         <v>41628</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="3" t="n">
+        <v>98</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>40880</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="4" t="n">
         <v>41618</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="3" t="n">
+      <c r="I2" s="4" t="n">
         <v>45270</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="J2" s="4" t="n">
         <v>41614</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>100</v>
       </c>
       <c r="L2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>999</v>
       </c>
       <c r="P2" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="R2" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="S2" s="0" t="s">
         <v>106</v>
       </c>
       <c r="T2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="Z2" s="3" t="n">
+      <c r="X2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB2" s="4" t="n">
         <v>41618</v>
       </c>
-      <c r="AA2" s="3" t="n">
+      <c r="AC2" s="4" t="n">
         <v>45270</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AD2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK2" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="AK2" s="0" t="s">
-        <v>114</v>
       </c>
       <c r="AL2" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="AM2" s="3" t="n">
+      <c r="AM2" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AO2" s="4" t="n">
         <v>41618</v>
       </c>
-      <c r="AN2" s="3" t="n">
+      <c r="AP2" s="4" t="n">
         <v>45270</v>
       </c>
-      <c r="AO2" s="0" t="s">
-        <v>110</v>
-      </c>
       <c r="AQ2" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="AR2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="AS2" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="AS2" s="0" t="s">
+      <c r="AT2" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="AT2" s="0" t="s">
+      <c r="AU2" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AV2" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="AV2" s="0" t="s">
+      <c r="AW2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AW2" s="0" t="s">
+      <c r="AX2" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="AX2" s="0" t="s">
-        <v>122</v>
       </c>
       <c r="AY2" s="0" t="s">
         <v>122</v>
       </c>
+      <c r="AZ2" s="0" t="s">
+        <v>123</v>
+      </c>
       <c r="BA2" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="BB2" s="0" t="s">
-        <v>124</v>
-      </c>
       <c r="BC2" s="0" t="s">
         <v>124</v>
+      </c>
+      <c r="BD2" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="BE2" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K7" s="0" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>